<commit_message>
[i18n] Implement locatable management strategy
</commit_message>
<xml_diff>
--- a/platform/microservices/blockchain-gateway-api/src/main/resources/i18n/translation_default.xlsx
+++ b/platform/microservices/blockchain-gateway-api/src/main/resources/i18n/translation_default.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssanchez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssanchez\Documents\trustCertificationSystemBlockchain\platform\microservices\blockchain-gateway-api\src\main\resources\i18n\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4575"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Cosechalia Platform" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>de_DE</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>Translation file uploaded correctly</t>
+  </si>
+  <si>
+    <t>user_id_not_valid</t>
+  </si>
+  <si>
+    <t>El identificador del usuario no es válido</t>
+  </si>
+  <si>
+    <t>The user identifier is not valid</t>
   </si>
 </sst>
 </file>
@@ -453,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -503,6 +512,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="4"/>

</xml_diff>